<commit_message>
Sottomissione risultati per wepacs, We BiNar S.r.l., 2.0
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#WEBINARSRLXX/We_BiNar_S.r.l/wepacs/2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#WEBINARSRLXX/We_BiNar_S.r.l/wepacs/2.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\WeBinar\wepacs\misc\FSE\GATEWAY\A1#111#WEBINARSRLXX\We_BiNar_S.r.l\wepacs\2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13C29B1-C3D8-4973-BBED-265AD2D3C4D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDEC31E-6027-40E1-B145-24B7A769A4E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="208">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -3362,9 +3362,7 @@
       <c r="J13" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="K13" s="35" t="s">
-        <v>62</v>
-      </c>
+      <c r="K13" s="35"/>
       <c r="L13" s="35"/>
       <c r="M13" s="35" t="s">
         <v>56</v>
@@ -3425,9 +3423,7 @@
       <c r="J14" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="K14" s="35" t="s">
-        <v>62</v>
-      </c>
+      <c r="K14" s="35"/>
       <c r="L14" s="35"/>
       <c r="M14" s="35" t="s">
         <v>56</v>
@@ -3488,9 +3484,7 @@
       <c r="J15" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="K15" s="35" t="s">
-        <v>62</v>
-      </c>
+      <c r="K15" s="35"/>
       <c r="L15" s="35"/>
       <c r="M15" s="35" t="s">
         <v>56</v>
@@ -3551,9 +3545,7 @@
       <c r="J16" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="K16" s="35" t="s">
-        <v>62</v>
-      </c>
+      <c r="K16" s="35"/>
       <c r="L16" s="35"/>
       <c r="M16" s="35" t="s">
         <v>56</v>
@@ -3614,9 +3606,7 @@
       <c r="J17" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="K17" s="35" t="s">
-        <v>62</v>
-      </c>
+      <c r="K17" s="35"/>
       <c r="L17" s="35"/>
       <c r="M17" s="35" t="s">
         <v>56</v>
@@ -3677,9 +3667,7 @@
       <c r="J18" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="K18" s="35" t="s">
-        <v>62</v>
-      </c>
+      <c r="K18" s="35"/>
       <c r="L18" s="35"/>
       <c r="M18" s="35" t="s">
         <v>56</v>
@@ -3740,9 +3728,7 @@
       <c r="J19" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="K19" s="35" t="s">
-        <v>62</v>
-      </c>
+      <c r="K19" s="35"/>
       <c r="L19" s="35"/>
       <c r="M19" s="35" t="s">
         <v>56</v>
@@ -3803,9 +3789,7 @@
       <c r="J20" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="K20" s="35" t="s">
-        <v>62</v>
-      </c>
+      <c r="K20" s="35"/>
       <c r="L20" s="35"/>
       <c r="M20" s="35" t="s">
         <v>56</v>
@@ -3866,9 +3850,7 @@
       <c r="J21" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="K21" s="35" t="s">
-        <v>62</v>
-      </c>
+      <c r="K21" s="35"/>
       <c r="L21" s="35"/>
       <c r="M21" s="35" t="s">
         <v>56</v>
@@ -3929,9 +3911,7 @@
       <c r="J22" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="K22" s="35" t="s">
-        <v>62</v>
-      </c>
+      <c r="K22" s="35"/>
       <c r="L22" s="35"/>
       <c r="M22" s="35" t="s">
         <v>56</v>
@@ -3992,9 +3972,7 @@
       <c r="J23" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="K23" s="35" t="s">
-        <v>62</v>
-      </c>
+      <c r="K23" s="35"/>
       <c r="L23" s="35"/>
       <c r="M23" s="35" t="s">
         <v>56</v>
@@ -4055,9 +4033,7 @@
       <c r="J24" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="K24" s="35" t="s">
-        <v>62</v>
-      </c>
+      <c r="K24" s="35"/>
       <c r="L24" s="35"/>
       <c r="M24" s="35" t="s">
         <v>56</v>
@@ -4118,9 +4094,7 @@
       <c r="J25" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="K25" s="35" t="s">
-        <v>62</v>
-      </c>
+      <c r="K25" s="35"/>
       <c r="L25" s="35"/>
       <c r="M25" s="35" t="s">
         <v>56</v>
@@ -4181,9 +4155,7 @@
       <c r="J26" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="K26" s="35" t="s">
-        <v>62</v>
-      </c>
+      <c r="K26" s="35"/>
       <c r="L26" s="35"/>
       <c r="M26" s="35" t="s">
         <v>56</v>
@@ -4244,9 +4216,7 @@
       <c r="J27" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="K27" s="35" t="s">
-        <v>62</v>
-      </c>
+      <c r="K27" s="35"/>
       <c r="L27" s="35"/>
       <c r="M27" s="35" t="s">
         <v>56</v>
@@ -4307,9 +4277,7 @@
       <c r="J28" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="K28" s="35" t="s">
-        <v>62</v>
-      </c>
+      <c r="K28" s="35"/>
       <c r="L28" s="35"/>
       <c r="M28" s="35" t="s">
         <v>56</v>
@@ -4370,9 +4338,7 @@
       <c r="J29" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="K29" s="35" t="s">
-        <v>62</v>
-      </c>
+      <c r="K29" s="35"/>
       <c r="L29" s="35"/>
       <c r="M29" s="35" t="s">
         <v>56</v>
@@ -4433,9 +4399,7 @@
       <c r="J30" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="K30" s="35" t="s">
-        <v>62</v>
-      </c>
+      <c r="K30" s="35"/>
       <c r="L30" s="35"/>
       <c r="M30" s="35"/>
       <c r="N30" s="35"/>
@@ -4482,9 +4446,7 @@
       <c r="J31" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="K31" s="35" t="s">
-        <v>62</v>
-      </c>
+      <c r="K31" s="35"/>
       <c r="L31" s="35"/>
       <c r="M31" s="35"/>
       <c r="N31" s="35"/>
@@ -4531,9 +4493,7 @@
       <c r="J32" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="K32" s="35" t="s">
-        <v>62</v>
-      </c>
+      <c r="K32" s="35"/>
       <c r="L32" s="35"/>
       <c r="M32" s="35" t="s">
         <v>56</v>
@@ -10357,18 +10317,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -10626,6 +10574,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -10636,23 +10596,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10671,6 +10614,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>

</xml_diff>